<commit_message>
fixing the style and option to add new records
</commit_message>
<xml_diff>
--- a/src/assets/MembershipData.xlsx
+++ b/src/assets/MembershipData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\tam-members\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9FDD01-39BA-4700-BFB1-AB3980B91A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01AE638B-538C-4C6D-A6F9-0872F936A722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{1F51C348-A47B-4F17-A7FA-BEAAD77C1C4F}"/>
   </bookViews>
@@ -2070,9 +2070,6 @@
     <t>Ganugapati</t>
   </si>
   <si>
-    <t>sridhar.ganugapati@gmail.com,sailakshmi670@gmail.com</t>
-  </si>
-  <si>
     <t>Sridharreddy</t>
   </si>
   <si>
@@ -2902,6 +2899,9 @@
   </si>
   <si>
     <t>Benevity</t>
+  </si>
+  <si>
+    <t>sridhar.ganugapati@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -3630,8 +3630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B3152D-0757-464D-9D51-AEB4CC777707}">
   <dimension ref="A1:I401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="D245" sqref="D245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -3969,7 +3969,7 @@
         <v>49</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -4015,7 +4015,7 @@
         <v>7</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -4153,7 +4153,7 @@
         <v>7</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
@@ -4176,7 +4176,7 @@
         <v>7</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -4245,7 +4245,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -4291,7 +4291,7 @@
         <v>7</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -4314,7 +4314,7 @@
         <v>49</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -4337,7 +4337,7 @@
         <v>49</v>
       </c>
       <c r="F30" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
@@ -4360,7 +4360,7 @@
         <v>7</v>
       </c>
       <c r="F31" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
@@ -4611,7 +4611,7 @@
         <v>7</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -4680,7 +4680,7 @@
         <v>7</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -4703,7 +4703,7 @@
         <v>18</v>
       </c>
       <c r="F46" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -4795,7 +4795,7 @@
         <v>18</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -5002,7 +5002,7 @@
         <v>7</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -5071,7 +5071,7 @@
         <v>18</v>
       </c>
       <c r="F62" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -5232,7 +5232,7 @@
         <v>7</v>
       </c>
       <c r="F69" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
@@ -5255,7 +5255,7 @@
         <v>18</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
@@ -5437,7 +5437,7 @@
         <v>7</v>
       </c>
       <c r="F78" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
@@ -5460,7 +5460,7 @@
         <v>49</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -5690,7 +5690,7 @@
         <v>7</v>
       </c>
       <c r="F89" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
@@ -5805,7 +5805,7 @@
         <v>18</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
@@ -5851,7 +5851,7 @@
         <v>18</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
@@ -5920,7 +5920,7 @@
         <v>7</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -6242,7 +6242,7 @@
         <v>18</v>
       </c>
       <c r="F113" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
@@ -6470,7 +6470,7 @@
         <v>18</v>
       </c>
       <c r="F123" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
@@ -6815,7 +6815,7 @@
         <v>18</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
@@ -6838,7 +6838,7 @@
         <v>49</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
@@ -6976,7 +6976,7 @@
         <v>7</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
@@ -7160,7 +7160,7 @@
         <v>18</v>
       </c>
       <c r="F153" s="8" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
@@ -7183,7 +7183,7 @@
         <v>18</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
@@ -7206,7 +7206,7 @@
         <v>7</v>
       </c>
       <c r="F155" s="25" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
@@ -7432,7 +7432,7 @@
         <v>7</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
@@ -7545,7 +7545,7 @@
         <v>18</v>
       </c>
       <c r="F170" s="36" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
@@ -7633,7 +7633,7 @@
         <v>18</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
@@ -7817,7 +7817,7 @@
         <v>18</v>
       </c>
       <c r="F182" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
@@ -8254,7 +8254,7 @@
         <v>18</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G201" s="2"/>
       <c r="H201" s="2"/>
@@ -8323,7 +8323,7 @@
         <v>18</v>
       </c>
       <c r="F204" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G204" s="2"/>
       <c r="H204" s="2"/>
@@ -8392,7 +8392,7 @@
         <v>18</v>
       </c>
       <c r="F207" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G207" s="2"/>
       <c r="H207" s="2"/>
@@ -8576,7 +8576,7 @@
         <v>7</v>
       </c>
       <c r="F215" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G215" s="2"/>
       <c r="H215" s="2"/>
@@ -8691,7 +8691,7 @@
         <v>18</v>
       </c>
       <c r="F220" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G220" s="2"/>
       <c r="H220" s="2"/>
@@ -8760,7 +8760,7 @@
         <v>7</v>
       </c>
       <c r="F223" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G223" s="2"/>
       <c r="H223" s="2"/>
@@ -8894,7 +8894,7 @@
         <v>18</v>
       </c>
       <c r="F229" s="36" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G229" s="2"/>
       <c r="H229" s="2"/>
@@ -8917,7 +8917,7 @@
         <v>7</v>
       </c>
       <c r="F230" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G230" s="2"/>
       <c r="H230" s="2"/>
@@ -8940,7 +8940,7 @@
         <v>7</v>
       </c>
       <c r="F231" s="9" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="G231" s="2"/>
       <c r="H231" s="2"/>
@@ -8963,7 +8963,7 @@
         <v>49</v>
       </c>
       <c r="F232" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G232" s="2"/>
       <c r="H232" s="2"/>
@@ -9032,7 +9032,7 @@
         <v>7</v>
       </c>
       <c r="F235" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G235" s="2"/>
       <c r="H235" s="2"/>
@@ -9193,7 +9193,7 @@
         <v>7</v>
       </c>
       <c r="F242" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G242" s="2"/>
       <c r="H242" s="2"/>
@@ -9383,15 +9383,15 @@
       <c r="H250" s="2"/>
       <c r="I250" s="2"/>
     </row>
-    <row r="251" spans="1:9" ht="27" x14ac:dyDescent="0.75">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A251" s="18" t="s">
         <v>677</v>
       </c>
       <c r="B251" s="18" t="s">
         <v>680</v>
       </c>
-      <c r="C251" s="19" t="s">
-        <v>681</v>
+      <c r="C251" s="13" t="s">
+        <v>958</v>
       </c>
       <c r="D251" s="8" t="s">
         <v>2</v>
@@ -9408,13 +9408,13 @@
     </row>
     <row r="252" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A252" s="5" t="s">
+        <v>681</v>
+      </c>
+      <c r="B252" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="B252" s="5" t="s">
+      <c r="C252" s="13" t="s">
         <v>683</v>
-      </c>
-      <c r="C252" s="13" t="s">
-        <v>684</v>
       </c>
       <c r="D252" s="14">
         <v>9016561287</v>
@@ -9431,13 +9431,13 @@
     </row>
     <row r="253" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A253" s="18" t="s">
+        <v>684</v>
+      </c>
+      <c r="B253" s="18" t="s">
         <v>685</v>
       </c>
-      <c r="B253" s="18" t="s">
+      <c r="C253" s="13" t="s">
         <v>686</v>
-      </c>
-      <c r="C253" s="13" t="s">
-        <v>687</v>
       </c>
       <c r="D253" s="61">
         <v>8622139394</v>
@@ -9454,13 +9454,13 @@
     </row>
     <row r="254" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A254" s="5" t="s">
+        <v>687</v>
+      </c>
+      <c r="B254" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="B254" s="5" t="s">
+      <c r="C254" s="19" t="s">
         <v>689</v>
-      </c>
-      <c r="C254" s="19" t="s">
-        <v>690</v>
       </c>
       <c r="D254" s="25">
         <v>2012183928</v>
@@ -9469,7 +9469,7 @@
         <v>7</v>
       </c>
       <c r="F254" s="25" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G254" s="2"/>
       <c r="H254" s="2"/>
@@ -9477,13 +9477,13 @@
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A255" s="18" t="s">
+        <v>690</v>
+      </c>
+      <c r="B255" s="18" t="s">
         <v>691</v>
       </c>
-      <c r="B255" s="18" t="s">
+      <c r="C255" s="19" t="s">
         <v>692</v>
-      </c>
-      <c r="C255" s="19" t="s">
-        <v>693</v>
       </c>
       <c r="D255" s="36">
         <v>9015383549</v>
@@ -9500,13 +9500,13 @@
     </row>
     <row r="256" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A256" s="5" t="s">
+        <v>693</v>
+      </c>
+      <c r="B256" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="B256" s="5" t="s">
+      <c r="C256" s="13" t="s">
         <v>695</v>
-      </c>
-      <c r="C256" s="13" t="s">
-        <v>696</v>
       </c>
       <c r="D256" s="8" t="s">
         <v>2</v>
@@ -9523,10 +9523,10 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A257" s="34" t="s">
+        <v>696</v>
+      </c>
+      <c r="B257" s="34" t="s">
         <v>697</v>
-      </c>
-      <c r="B257" s="34" t="s">
-        <v>698</v>
       </c>
       <c r="C257" s="19" t="s">
         <v>2</v>
@@ -9546,13 +9546,13 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A258" s="18" t="s">
+        <v>698</v>
+      </c>
+      <c r="B258" s="18" t="s">
         <v>699</v>
       </c>
-      <c r="B258" s="18" t="s">
+      <c r="C258" s="19" t="s">
         <v>700</v>
-      </c>
-      <c r="C258" s="19" t="s">
-        <v>701</v>
       </c>
       <c r="D258" s="8" t="s">
         <v>2</v>
@@ -9569,13 +9569,13 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A259" s="62" t="s">
+        <v>701</v>
+      </c>
+      <c r="B259" s="62" t="s">
         <v>702</v>
       </c>
-      <c r="B259" s="62" t="s">
+      <c r="C259" s="19" t="s">
         <v>703</v>
-      </c>
-      <c r="C259" s="19" t="s">
-        <v>704</v>
       </c>
       <c r="D259" s="9">
         <v>4792680441</v>
@@ -9584,7 +9584,7 @@
         <v>7</v>
       </c>
       <c r="F259" s="9" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="G259" s="2"/>
       <c r="H259" s="2"/>
@@ -9592,13 +9592,13 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A260" s="18" t="s">
+        <v>704</v>
+      </c>
+      <c r="B260" s="18" t="s">
         <v>705</v>
       </c>
-      <c r="B260" s="18" t="s">
+      <c r="C260" s="19" t="s">
         <v>706</v>
-      </c>
-      <c r="C260" s="19" t="s">
-        <v>707</v>
       </c>
       <c r="D260" s="14">
         <v>9019075978</v>
@@ -9615,13 +9615,13 @@
     </row>
     <row r="261" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A261" s="5" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B261" s="5" t="s">
+        <v>707</v>
+      </c>
+      <c r="C261" s="13" t="s">
         <v>708</v>
-      </c>
-      <c r="C261" s="13" t="s">
-        <v>709</v>
       </c>
       <c r="D261" s="8" t="s">
         <v>2</v>
@@ -9638,13 +9638,13 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A262" s="26" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B262" s="26" t="s">
+        <v>709</v>
+      </c>
+      <c r="C262" s="13" t="s">
         <v>710</v>
-      </c>
-      <c r="C262" s="13" t="s">
-        <v>711</v>
       </c>
       <c r="D262" s="8" t="s">
         <v>2</v>
@@ -9661,10 +9661,10 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A263" s="18" t="s">
+        <v>711</v>
+      </c>
+      <c r="B263" s="18" t="s">
         <v>712</v>
-      </c>
-      <c r="B263" s="18" t="s">
-        <v>713</v>
       </c>
       <c r="C263" s="19" t="s">
         <v>2</v>
@@ -9684,13 +9684,13 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A264" s="31" t="s">
+        <v>713</v>
+      </c>
+      <c r="B264" s="32" t="s">
         <v>714</v>
       </c>
-      <c r="B264" s="32" t="s">
+      <c r="C264" s="32" t="s">
         <v>715</v>
-      </c>
-      <c r="C264" s="32" t="s">
-        <v>716</v>
       </c>
       <c r="D264" s="32"/>
       <c r="E264" s="31" t="s">
@@ -9705,13 +9705,13 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A265" s="29" t="s">
+        <v>716</v>
+      </c>
+      <c r="B265" s="29" t="s">
         <v>717</v>
       </c>
-      <c r="B265" s="29" t="s">
+      <c r="C265" s="13" t="s">
         <v>718</v>
-      </c>
-      <c r="C265" s="13" t="s">
-        <v>719</v>
       </c>
       <c r="D265" s="8" t="s">
         <v>2</v>
@@ -9728,13 +9728,13 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A266" s="18" t="s">
+        <v>719</v>
+      </c>
+      <c r="B266" s="18" t="s">
         <v>720</v>
       </c>
-      <c r="B266" s="18" t="s">
+      <c r="C266" s="13" t="s">
         <v>721</v>
-      </c>
-      <c r="C266" s="13" t="s">
-        <v>722</v>
       </c>
       <c r="D266" s="8">
         <v>2017746474</v>
@@ -9751,13 +9751,13 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A267" s="34" t="s">
+        <v>722</v>
+      </c>
+      <c r="B267" s="34" t="s">
         <v>723</v>
       </c>
-      <c r="B267" s="34" t="s">
+      <c r="C267" s="19" t="s">
         <v>724</v>
-      </c>
-      <c r="C267" s="19" t="s">
-        <v>725</v>
       </c>
       <c r="D267" s="8" t="s">
         <v>2</v>
@@ -9774,7 +9774,7 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A268" s="5" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B268" s="5" t="s">
         <v>2</v>
@@ -9797,7 +9797,7 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A269" s="32" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B269" s="32"/>
       <c r="C269" s="32"/>
@@ -9814,7 +9814,7 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A270" s="32" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B270" s="32"/>
       <c r="C270" s="32"/>
@@ -9831,13 +9831,13 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A271" s="31" t="s">
+        <v>728</v>
+      </c>
+      <c r="B271" s="31" t="s">
         <v>729</v>
       </c>
-      <c r="B271" s="31" t="s">
+      <c r="C271" s="31" t="s">
         <v>730</v>
-      </c>
-      <c r="C271" s="31" t="s">
-        <v>731</v>
       </c>
       <c r="D271" s="32" t="s">
         <v>2</v>
@@ -9854,11 +9854,11 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A272" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B272" s="5" t="s">
         <v>732</v>
       </c>
-      <c r="B272" s="5" t="s">
-        <v>733</v>
-      </c>
       <c r="C272" s="19" t="s">
         <v>2</v>
       </c>
@@ -9869,7 +9869,7 @@
         <v>7</v>
       </c>
       <c r="F272" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G272" s="2"/>
       <c r="H272" s="2"/>
@@ -9877,10 +9877,10 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A273" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B273" s="5" t="s">
         <v>734</v>
-      </c>
-      <c r="B273" s="5" t="s">
-        <v>735</v>
       </c>
       <c r="C273" s="5" t="s">
         <v>2</v>
@@ -9900,22 +9900,22 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A274" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="B274" s="5" t="s">
         <v>736</v>
       </c>
-      <c r="B274" s="5" t="s">
+      <c r="C274" s="5" t="s">
         <v>737</v>
       </c>
-      <c r="C274" s="5" t="s">
+      <c r="D274" s="9" t="s">
         <v>738</v>
       </c>
-      <c r="D274" s="9" t="s">
-        <v>739</v>
-      </c>
       <c r="E274" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F274" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G274" s="2"/>
       <c r="H274" s="2"/>
@@ -9923,13 +9923,13 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A275" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="B275" s="5" t="s">
         <v>740</v>
       </c>
-      <c r="B275" s="5" t="s">
+      <c r="C275" s="5" t="s">
         <v>741</v>
-      </c>
-      <c r="C275" s="5" t="s">
-        <v>742</v>
       </c>
       <c r="D275" s="6" t="s">
         <v>2</v>
@@ -9946,10 +9946,10 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A276" s="18" t="s">
+        <v>742</v>
+      </c>
+      <c r="B276" s="18" t="s">
         <v>743</v>
-      </c>
-      <c r="B276" s="18" t="s">
-        <v>744</v>
       </c>
       <c r="C276" s="19" t="s">
         <v>2</v>
@@ -9969,13 +9969,13 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A277" s="26" t="s">
+        <v>744</v>
+      </c>
+      <c r="B277" s="26" t="s">
         <v>745</v>
       </c>
-      <c r="B277" s="26" t="s">
+      <c r="C277" s="13" t="s">
         <v>746</v>
-      </c>
-      <c r="C277" s="13" t="s">
-        <v>747</v>
       </c>
       <c r="D277" s="8" t="s">
         <v>2</v>
@@ -9992,10 +9992,10 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A278" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="B278" s="5" t="s">
         <v>748</v>
-      </c>
-      <c r="B278" s="5" t="s">
-        <v>749</v>
       </c>
       <c r="C278" s="5" t="s">
         <v>2</v>
@@ -10015,13 +10015,13 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A279" s="34" t="s">
+        <v>749</v>
+      </c>
+      <c r="B279" s="34" t="s">
         <v>750</v>
       </c>
-      <c r="B279" s="34" t="s">
+      <c r="C279" s="19" t="s">
         <v>751</v>
-      </c>
-      <c r="C279" s="19" t="s">
-        <v>752</v>
       </c>
       <c r="D279" s="8" t="s">
         <v>2</v>
@@ -10038,13 +10038,13 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A280" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="B280" s="26" t="s">
         <v>753</v>
       </c>
-      <c r="B280" s="26" t="s">
+      <c r="C280" s="13" t="s">
         <v>754</v>
-      </c>
-      <c r="C280" s="13" t="s">
-        <v>755</v>
       </c>
       <c r="D280" s="8" t="s">
         <v>2</v>
@@ -10061,10 +10061,10 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A281" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B281" s="5" t="s">
         <v>756</v>
-      </c>
-      <c r="B281" s="5" t="s">
-        <v>757</v>
       </c>
       <c r="C281" s="19" t="s">
         <v>2</v>
@@ -10076,7 +10076,7 @@
         <v>18</v>
       </c>
       <c r="F281" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G281" s="2"/>
       <c r="H281" s="2"/>
@@ -10084,13 +10084,13 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A282" s="18" t="s">
+        <v>757</v>
+      </c>
+      <c r="B282" s="18" t="s">
         <v>758</v>
       </c>
-      <c r="B282" s="18" t="s">
+      <c r="C282" s="19" t="s">
         <v>759</v>
-      </c>
-      <c r="C282" s="19" t="s">
-        <v>760</v>
       </c>
       <c r="D282" s="8" t="s">
         <v>2</v>
@@ -10107,13 +10107,13 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A283" s="53" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B283" s="53" t="s">
         <v>399</v>
       </c>
       <c r="C283" s="19" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D283" s="6">
         <v>2243580920</v>
@@ -10130,13 +10130,13 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A284" s="18" t="s">
+        <v>761</v>
+      </c>
+      <c r="B284" s="18" t="s">
         <v>762</v>
       </c>
-      <c r="B284" s="18" t="s">
+      <c r="C284" s="19" t="s">
         <v>763</v>
-      </c>
-      <c r="C284" s="19" t="s">
-        <v>764</v>
       </c>
       <c r="D284" s="14">
         <v>5512635799</v>
@@ -10145,7 +10145,7 @@
         <v>18</v>
       </c>
       <c r="F284" s="14" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="G284" s="2"/>
       <c r="H284" s="2"/>
@@ -10153,13 +10153,13 @@
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A285" s="18" t="s">
+        <v>764</v>
+      </c>
+      <c r="B285" s="18" t="s">
         <v>765</v>
       </c>
-      <c r="B285" s="18" t="s">
+      <c r="C285" s="19" t="s">
         <v>766</v>
-      </c>
-      <c r="C285" s="19" t="s">
-        <v>767</v>
       </c>
       <c r="D285" s="16">
         <v>9013182909</v>
@@ -10176,13 +10176,13 @@
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A286" s="5" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B286" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="C286" s="5" t="s">
         <v>768</v>
-      </c>
-      <c r="C286" s="5" t="s">
-        <v>769</v>
       </c>
       <c r="D286" s="9">
         <v>9015671292</v>
@@ -10191,7 +10191,7 @@
         <v>7</v>
       </c>
       <c r="F286" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G286" s="2"/>
       <c r="H286" s="2"/>
@@ -10199,13 +10199,13 @@
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A287" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="B287" s="5" t="s">
         <v>770</v>
       </c>
-      <c r="B287" s="5" t="s">
+      <c r="C287" s="19" t="s">
         <v>771</v>
-      </c>
-      <c r="C287" s="19" t="s">
-        <v>772</v>
       </c>
       <c r="D287" s="8">
         <v>9014094813</v>
@@ -10214,7 +10214,7 @@
         <v>18</v>
       </c>
       <c r="F287" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G287" s="2"/>
       <c r="H287" s="2"/>
@@ -10222,10 +10222,10 @@
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A288" s="18" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B288" s="18" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C288" s="19" t="s">
         <v>2</v>
@@ -10245,13 +10245,13 @@
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A289" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="B289" s="5" t="s">
         <v>774</v>
       </c>
-      <c r="B289" s="5" t="s">
+      <c r="C289" s="13" t="s">
         <v>775</v>
-      </c>
-      <c r="C289" s="13" t="s">
-        <v>776</v>
       </c>
       <c r="D289" s="8" t="s">
         <v>2</v>
@@ -10268,10 +10268,10 @@
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A290" s="34" t="s">
+        <v>776</v>
+      </c>
+      <c r="B290" s="34" t="s">
         <v>777</v>
-      </c>
-      <c r="B290" s="34" t="s">
-        <v>778</v>
       </c>
       <c r="C290" s="19" t="s">
         <v>2</v>
@@ -10291,13 +10291,13 @@
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A291" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="B291" s="5" t="s">
         <v>779</v>
       </c>
-      <c r="B291" s="5" t="s">
+      <c r="C291" s="5" t="s">
         <v>780</v>
-      </c>
-      <c r="C291" s="5" t="s">
-        <v>781</v>
       </c>
       <c r="D291" s="8" t="s">
         <v>2</v>
@@ -10314,13 +10314,13 @@
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A292" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="B292" s="5" t="s">
         <v>782</v>
       </c>
-      <c r="B292" s="5" t="s">
+      <c r="C292" s="19" t="s">
         <v>783</v>
-      </c>
-      <c r="C292" s="19" t="s">
-        <v>784</v>
       </c>
       <c r="D292" s="16">
         <v>9015187539</v>
@@ -10329,7 +10329,7 @@
         <v>18</v>
       </c>
       <c r="F292" s="14" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G292" s="2"/>
       <c r="H292" s="2"/>
@@ -10337,11 +10337,11 @@
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A293" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B293" s="5" t="s">
         <v>785</v>
       </c>
-      <c r="B293" s="5" t="s">
-        <v>786</v>
-      </c>
       <c r="C293" s="19" t="s">
         <v>2</v>
       </c>
@@ -10352,7 +10352,7 @@
         <v>7</v>
       </c>
       <c r="F293" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G293" s="2"/>
       <c r="H293" s="2"/>
@@ -10360,10 +10360,10 @@
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A294" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="B294" s="5" t="s">
         <v>787</v>
-      </c>
-      <c r="B294" s="5" t="s">
-        <v>788</v>
       </c>
       <c r="C294" s="19" t="s">
         <v>2</v>
@@ -10375,7 +10375,7 @@
         <v>49</v>
       </c>
       <c r="F294" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G294" s="2"/>
       <c r="H294" s="2"/>
@@ -10383,13 +10383,13 @@
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A295" s="18" t="s">
+        <v>788</v>
+      </c>
+      <c r="B295" s="18" t="s">
         <v>789</v>
       </c>
-      <c r="B295" s="18" t="s">
+      <c r="C295" s="19" t="s">
         <v>790</v>
-      </c>
-      <c r="C295" s="19" t="s">
-        <v>791</v>
       </c>
       <c r="D295" s="14">
         <v>9012830473</v>
@@ -10406,13 +10406,13 @@
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A296" s="18" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B296" s="18" t="s">
+        <v>791</v>
+      </c>
+      <c r="C296" s="19" t="s">
         <v>792</v>
-      </c>
-      <c r="C296" s="19" t="s">
-        <v>793</v>
       </c>
       <c r="D296" s="8">
         <v>4792766087</v>
@@ -10429,13 +10429,13 @@
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A297" s="18" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B297" s="18" t="s">
+        <v>793</v>
+      </c>
+      <c r="C297" s="13" t="s">
         <v>794</v>
-      </c>
-      <c r="C297" s="13" t="s">
-        <v>795</v>
       </c>
       <c r="D297" s="14">
         <v>5189158066</v>
@@ -10452,13 +10452,13 @@
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A298" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="B298" s="5" t="s">
         <v>796</v>
       </c>
-      <c r="B298" s="5" t="s">
+      <c r="C298" s="13" t="s">
         <v>797</v>
-      </c>
-      <c r="C298" s="13" t="s">
-        <v>798</v>
       </c>
       <c r="D298" s="8" t="s">
         <v>2</v>
@@ -10475,13 +10475,13 @@
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A299" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B299" s="5" t="s">
         <v>799</v>
       </c>
-      <c r="B299" s="5" t="s">
+      <c r="C299" s="13" t="s">
         <v>800</v>
-      </c>
-      <c r="C299" s="13" t="s">
-        <v>801</v>
       </c>
       <c r="D299" s="8">
         <v>9013366583</v>
@@ -10490,7 +10490,7 @@
         <v>7</v>
       </c>
       <c r="F299" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G299" s="2"/>
       <c r="H299" s="2"/>
@@ -10498,10 +10498,10 @@
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A300" s="43" t="s">
+        <v>801</v>
+      </c>
+      <c r="B300" s="43" t="s">
         <v>802</v>
-      </c>
-      <c r="B300" s="43" t="s">
-        <v>803</v>
       </c>
       <c r="C300" s="43" t="s">
         <v>2</v>
@@ -10521,10 +10521,10 @@
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A301" s="41" t="s">
+        <v>803</v>
+      </c>
+      <c r="B301" s="41" t="s">
         <v>804</v>
-      </c>
-      <c r="B301" s="41" t="s">
-        <v>805</v>
       </c>
       <c r="C301" s="41" t="s">
         <v>2</v>
@@ -10544,13 +10544,13 @@
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A302" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B302" s="5" t="s">
         <v>806</v>
       </c>
-      <c r="B302" s="5" t="s">
+      <c r="C302" s="5" t="s">
         <v>807</v>
-      </c>
-      <c r="C302" s="5" t="s">
-        <v>808</v>
       </c>
       <c r="D302" s="6" t="s">
         <v>2</v>
@@ -10567,10 +10567,10 @@
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A303" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="B303" s="5" t="s">
         <v>809</v>
-      </c>
-      <c r="B303" s="5" t="s">
-        <v>810</v>
       </c>
       <c r="C303" s="19" t="s">
         <v>2</v>
@@ -10590,10 +10590,10 @@
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A304" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B304" s="5" t="s">
         <v>811</v>
-      </c>
-      <c r="B304" s="5" t="s">
-        <v>812</v>
       </c>
       <c r="C304" s="5" t="s">
         <v>2</v>
@@ -10613,13 +10613,13 @@
     </row>
     <row r="305" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A305" s="18" t="s">
+        <v>812</v>
+      </c>
+      <c r="B305" s="18" t="s">
         <v>813</v>
       </c>
-      <c r="B305" s="18" t="s">
+      <c r="C305" s="19" t="s">
         <v>814</v>
-      </c>
-      <c r="C305" s="19" t="s">
-        <v>815</v>
       </c>
       <c r="D305" s="16">
         <v>9012301245</v>
@@ -10636,10 +10636,10 @@
     </row>
     <row r="306" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A306" s="18" t="s">
+        <v>815</v>
+      </c>
+      <c r="B306" s="18" t="s">
         <v>816</v>
-      </c>
-      <c r="B306" s="18" t="s">
-        <v>817</v>
       </c>
       <c r="C306" s="19" t="s">
         <v>2</v>
@@ -10659,13 +10659,13 @@
     </row>
     <row r="307" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A307" s="5" t="s">
+        <v>817</v>
+      </c>
+      <c r="B307" s="5" t="s">
         <v>818</v>
       </c>
-      <c r="B307" s="5" t="s">
+      <c r="C307" s="19" t="s">
         <v>819</v>
-      </c>
-      <c r="C307" s="19" t="s">
-        <v>820</v>
       </c>
       <c r="D307" s="8" t="s">
         <v>2</v>
@@ -10682,13 +10682,13 @@
     </row>
     <row r="308" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A308" s="26" t="s">
+        <v>820</v>
+      </c>
+      <c r="B308" s="26" t="s">
         <v>821</v>
       </c>
-      <c r="B308" s="26" t="s">
+      <c r="C308" s="13" t="s">
         <v>822</v>
-      </c>
-      <c r="C308" s="13" t="s">
-        <v>823</v>
       </c>
       <c r="D308" s="8" t="s">
         <v>2</v>
@@ -10697,7 +10697,7 @@
         <v>60</v>
       </c>
       <c r="F308" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G308" s="2"/>
       <c r="H308" s="2"/>
@@ -10705,13 +10705,13 @@
     </row>
     <row r="309" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A309" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="B309" s="5" t="s">
         <v>824</v>
       </c>
-      <c r="B309" s="5" t="s">
+      <c r="C309" s="19" t="s">
         <v>825</v>
-      </c>
-      <c r="C309" s="19" t="s">
-        <v>826</v>
       </c>
       <c r="D309" s="11">
         <v>4088937553</v>
@@ -10728,13 +10728,13 @@
     </row>
     <row r="310" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A310" s="5" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B310" s="5" t="s">
+        <v>826</v>
+      </c>
+      <c r="C310" s="19" t="s">
         <v>827</v>
-      </c>
-      <c r="C310" s="19" t="s">
-        <v>828</v>
       </c>
       <c r="D310" s="8">
         <v>9018601788</v>
@@ -10743,7 +10743,7 @@
         <v>18</v>
       </c>
       <c r="F310" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G310" s="2"/>
       <c r="H310" s="2"/>
@@ -10751,10 +10751,10 @@
     </row>
     <row r="311" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A311" s="18" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="B311" s="18" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C311" s="19" t="s">
         <v>2</v>
@@ -10774,13 +10774,13 @@
     </row>
     <row r="312" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A312" s="5" t="s">
+        <v>829</v>
+      </c>
+      <c r="B312" s="5" t="s">
         <v>830</v>
       </c>
-      <c r="B312" s="5" t="s">
+      <c r="C312" s="5" t="s">
         <v>831</v>
-      </c>
-      <c r="C312" s="5" t="s">
-        <v>832</v>
       </c>
       <c r="D312" s="8">
         <v>9734528251</v>
@@ -10797,10 +10797,10 @@
     </row>
     <row r="313" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A313" s="5" t="s">
+        <v>832</v>
+      </c>
+      <c r="B313" s="5" t="s">
         <v>833</v>
-      </c>
-      <c r="B313" s="5" t="s">
-        <v>834</v>
       </c>
       <c r="C313" s="19" t="s">
         <v>2</v>
@@ -10812,7 +10812,7 @@
         <v>18</v>
       </c>
       <c r="F313" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G313" s="2"/>
       <c r="H313" s="2"/>
@@ -10820,10 +10820,10 @@
     </row>
     <row r="314" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A314" s="18" t="s">
+        <v>834</v>
+      </c>
+      <c r="B314" s="18" t="s">
         <v>835</v>
-      </c>
-      <c r="B314" s="18" t="s">
-        <v>836</v>
       </c>
       <c r="C314" s="19" t="s">
         <v>2</v>
@@ -10843,13 +10843,13 @@
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A315" s="18" t="s">
+        <v>836</v>
+      </c>
+      <c r="B315" s="18" t="s">
         <v>837</v>
       </c>
-      <c r="B315" s="18" t="s">
+      <c r="C315" s="13" t="s">
         <v>838</v>
-      </c>
-      <c r="C315" s="13" t="s">
-        <v>839</v>
       </c>
       <c r="D315" s="8">
         <v>9174421560</v>
@@ -10866,11 +10866,11 @@
     </row>
     <row r="316" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A316" s="33" t="s">
+        <v>839</v>
+      </c>
+      <c r="B316" s="34" t="s">
         <v>840</v>
       </c>
-      <c r="B316" s="34" t="s">
-        <v>841</v>
-      </c>
       <c r="C316" s="19" t="s">
         <v>2</v>
       </c>
@@ -10881,7 +10881,7 @@
         <v>7</v>
       </c>
       <c r="F316" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G316" s="2"/>
       <c r="H316" s="2"/>
@@ -10889,10 +10889,10 @@
     </row>
     <row r="317" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A317" s="18" t="s">
+        <v>841</v>
+      </c>
+      <c r="B317" s="18" t="s">
         <v>842</v>
-      </c>
-      <c r="B317" s="18" t="s">
-        <v>843</v>
       </c>
       <c r="C317" s="19" t="s">
         <v>2</v>
@@ -10912,13 +10912,13 @@
     </row>
     <row r="318" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A318" s="34" t="s">
+        <v>843</v>
+      </c>
+      <c r="B318" s="34" t="s">
         <v>844</v>
       </c>
-      <c r="B318" s="34" t="s">
+      <c r="C318" s="13" t="s">
         <v>845</v>
-      </c>
-      <c r="C318" s="13" t="s">
-        <v>846</v>
       </c>
       <c r="D318" s="8">
         <v>2292961363</v>
@@ -10935,13 +10935,13 @@
     </row>
     <row r="319" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A319" s="18" t="s">
+        <v>846</v>
+      </c>
+      <c r="B319" s="18" t="s">
         <v>847</v>
       </c>
-      <c r="B319" s="18" t="s">
+      <c r="C319" s="19" t="s">
         <v>848</v>
-      </c>
-      <c r="C319" s="19" t="s">
-        <v>849</v>
       </c>
       <c r="D319" s="8" t="s">
         <v>2</v>
@@ -10958,13 +10958,13 @@
     </row>
     <row r="320" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A320" s="5" t="s">
+        <v>849</v>
+      </c>
+      <c r="B320" s="5" t="s">
         <v>850</v>
       </c>
-      <c r="B320" s="5" t="s">
+      <c r="C320" s="13" t="s">
         <v>851</v>
-      </c>
-      <c r="C320" s="13" t="s">
-        <v>852</v>
       </c>
       <c r="D320" s="8">
         <v>9016923537</v>
@@ -10973,7 +10973,7 @@
         <v>7</v>
       </c>
       <c r="F320" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G320" s="2"/>
       <c r="H320" s="2"/>
@@ -10981,13 +10981,13 @@
     </row>
     <row r="321" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A321" s="5" t="s">
+        <v>852</v>
+      </c>
+      <c r="B321" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="B321" s="5" t="s">
+      <c r="C321" s="13" t="s">
         <v>854</v>
-      </c>
-      <c r="C321" s="13" t="s">
-        <v>855</v>
       </c>
       <c r="D321" s="8">
         <v>9452788304</v>
@@ -11004,13 +11004,13 @@
     </row>
     <row r="322" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A322" s="5" t="s">
+        <v>855</v>
+      </c>
+      <c r="B322" s="5" t="s">
         <v>856</v>
       </c>
-      <c r="B322" s="5" t="s">
+      <c r="C322" s="19" t="s">
         <v>857</v>
-      </c>
-      <c r="C322" s="19" t="s">
-        <v>858</v>
       </c>
       <c r="D322" s="22" t="s">
         <v>2</v>
@@ -11027,13 +11027,13 @@
     </row>
     <row r="323" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A323" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B323" s="5" t="s">
+        <v>858</v>
+      </c>
+      <c r="C323" s="5" t="s">
         <v>859</v>
-      </c>
-      <c r="C323" s="5" t="s">
-        <v>860</v>
       </c>
       <c r="D323" s="8">
         <v>9014943249</v>
@@ -11050,10 +11050,10 @@
     </row>
     <row r="324" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A324" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B324" s="5" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C324" s="5" t="s">
         <v>2</v>
@@ -11065,7 +11065,7 @@
         <v>18</v>
       </c>
       <c r="F324" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G324" s="2"/>
       <c r="H324" s="2"/>
@@ -11073,13 +11073,13 @@
     </row>
     <row r="325" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A325" s="5" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B325" s="5" t="s">
         <v>536</v>
       </c>
       <c r="C325" s="5" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="D325" s="8" t="s">
         <v>2</v>
@@ -11088,7 +11088,7 @@
         <v>18</v>
       </c>
       <c r="F325" s="8" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G325" s="2"/>
       <c r="H325" s="2"/>
@@ -11096,13 +11096,13 @@
     </row>
     <row r="326" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A326" s="18" t="s">
+        <v>862</v>
+      </c>
+      <c r="B326" s="18" t="s">
         <v>863</v>
       </c>
-      <c r="B326" s="18" t="s">
+      <c r="C326" s="19" t="s">
         <v>864</v>
-      </c>
-      <c r="C326" s="19" t="s">
-        <v>865</v>
       </c>
       <c r="D326" s="15">
         <v>9014688754</v>
@@ -11119,13 +11119,13 @@
     </row>
     <row r="327" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A327" s="5" t="s">
+        <v>865</v>
+      </c>
+      <c r="B327" s="5" t="s">
         <v>866</v>
       </c>
-      <c r="B327" s="5" t="s">
+      <c r="C327" s="5" t="s">
         <v>867</v>
-      </c>
-      <c r="C327" s="5" t="s">
-        <v>868</v>
       </c>
       <c r="D327" s="8">
         <v>9014719225</v>
@@ -11142,13 +11142,13 @@
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A328" s="18" t="s">
+        <v>868</v>
+      </c>
+      <c r="B328" s="18" t="s">
         <v>869</v>
       </c>
-      <c r="B328" s="18" t="s">
+      <c r="C328" s="13" t="s">
         <v>870</v>
-      </c>
-      <c r="C328" s="13" t="s">
-        <v>871</v>
       </c>
       <c r="D328" s="8" t="s">
         <v>2</v>
@@ -11157,7 +11157,7 @@
         <v>18</v>
       </c>
       <c r="F328" s="25" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="G328" s="2"/>
       <c r="H328" s="2"/>
@@ -11165,10 +11165,10 @@
     </row>
     <row r="329" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A329" s="18" t="s">
+        <v>871</v>
+      </c>
+      <c r="B329" s="18" t="s">
         <v>872</v>
-      </c>
-      <c r="B329" s="18" t="s">
-        <v>873</v>
       </c>
       <c r="C329" s="19" t="s">
         <v>2</v>
@@ -11188,13 +11188,13 @@
     </row>
     <row r="330" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A330" s="24" t="s">
+        <v>873</v>
+      </c>
+      <c r="B330" s="24" t="s">
         <v>874</v>
       </c>
-      <c r="B330" s="24" t="s">
+      <c r="C330" s="19" t="s">
         <v>875</v>
-      </c>
-      <c r="C330" s="19" t="s">
-        <v>876</v>
       </c>
       <c r="D330" s="15">
         <v>8607185376</v>
@@ -11211,13 +11211,13 @@
     </row>
     <row r="331" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A331" s="18" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="B331" s="18" t="s">
+        <v>876</v>
+      </c>
+      <c r="C331" s="19" t="s">
         <v>877</v>
-      </c>
-      <c r="C331" s="19" t="s">
-        <v>878</v>
       </c>
       <c r="D331" s="36">
         <v>9019108065</v>
@@ -11234,10 +11234,10 @@
     </row>
     <row r="332" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A332" s="5" t="s">
+        <v>878</v>
+      </c>
+      <c r="B332" s="5" t="s">
         <v>879</v>
-      </c>
-      <c r="B332" s="5" t="s">
-        <v>880</v>
       </c>
       <c r="C332" s="19" t="s">
         <v>2</v>
@@ -11257,13 +11257,13 @@
     </row>
     <row r="333" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A333" s="5" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B333" s="5" t="s">
+        <v>880</v>
+      </c>
+      <c r="C333" s="5" t="s">
         <v>881</v>
-      </c>
-      <c r="C333" s="5" t="s">
-        <v>882</v>
       </c>
       <c r="D333" s="8">
         <v>2407010047</v>
@@ -11280,13 +11280,13 @@
     </row>
     <row r="334" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A334" s="18" t="s">
+        <v>882</v>
+      </c>
+      <c r="B334" s="18" t="s">
         <v>883</v>
       </c>
-      <c r="B334" s="18" t="s">
+      <c r="C334" s="13" t="s">
         <v>884</v>
-      </c>
-      <c r="C334" s="13" t="s">
-        <v>885</v>
       </c>
       <c r="D334" s="36">
         <v>7347408954</v>
@@ -11303,13 +11303,13 @@
     </row>
     <row r="335" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A335" s="5" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B335" s="5" t="s">
+        <v>885</v>
+      </c>
+      <c r="C335" s="13" t="s">
         <v>886</v>
-      </c>
-      <c r="C335" s="13" t="s">
-        <v>887</v>
       </c>
       <c r="D335" s="8">
         <v>9016512460</v>
@@ -11318,7 +11318,7 @@
         <v>18</v>
       </c>
       <c r="F335" s="8" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="G335" s="2"/>
       <c r="H335" s="2"/>
@@ -11326,16 +11326,16 @@
     </row>
     <row r="336" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A336" s="5" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B336" s="5" t="s">
+        <v>887</v>
+      </c>
+      <c r="C336" s="5" t="s">
         <v>888</v>
       </c>
-      <c r="C336" s="5" t="s">
+      <c r="D336" s="8" t="s">
         <v>889</v>
-      </c>
-      <c r="D336" s="8" t="s">
-        <v>890</v>
       </c>
       <c r="E336" s="8" t="s">
         <v>7</v>
@@ -11349,13 +11349,13 @@
     </row>
     <row r="337" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A337" s="34" t="s">
+        <v>890</v>
+      </c>
+      <c r="B337" s="34" t="s">
         <v>891</v>
       </c>
-      <c r="B337" s="34" t="s">
+      <c r="C337" s="19" t="s">
         <v>892</v>
-      </c>
-      <c r="C337" s="19" t="s">
-        <v>893</v>
       </c>
       <c r="D337" s="8" t="s">
         <v>2</v>
@@ -11372,10 +11372,10 @@
     </row>
     <row r="338" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A338" s="18" t="s">
+        <v>893</v>
+      </c>
+      <c r="B338" s="18" t="s">
         <v>894</v>
-      </c>
-      <c r="B338" s="18" t="s">
-        <v>895</v>
       </c>
       <c r="C338" s="19" t="s">
         <v>2</v>
@@ -11395,13 +11395,13 @@
     </row>
     <row r="339" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A339" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="B339" s="5" t="s">
         <v>896</v>
       </c>
-      <c r="B339" s="5" t="s">
+      <c r="C339" s="13" t="s">
         <v>897</v>
-      </c>
-      <c r="C339" s="13" t="s">
-        <v>898</v>
       </c>
       <c r="D339" s="8" t="s">
         <v>2</v>
@@ -11418,13 +11418,13 @@
     </row>
     <row r="340" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A340" s="7" t="s">
+        <v>898</v>
+      </c>
+      <c r="B340" s="7" t="s">
         <v>899</v>
       </c>
-      <c r="B340" s="7" t="s">
+      <c r="C340" s="7" t="s">
         <v>900</v>
-      </c>
-      <c r="C340" s="7" t="s">
-        <v>901</v>
       </c>
       <c r="D340" s="32"/>
       <c r="E340" s="35" t="s">
@@ -11439,13 +11439,13 @@
     </row>
     <row r="341" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A341" s="5" t="s">
+        <v>901</v>
+      </c>
+      <c r="B341" s="5" t="s">
         <v>902</v>
       </c>
-      <c r="B341" s="5" t="s">
+      <c r="C341" s="5" t="s">
         <v>903</v>
-      </c>
-      <c r="C341" s="5" t="s">
-        <v>904</v>
       </c>
       <c r="D341" s="8">
         <v>2019697241</v>
@@ -11462,13 +11462,13 @@
     </row>
     <row r="342" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A342" s="32" t="s">
+        <v>904</v>
+      </c>
+      <c r="B342" s="32" t="s">
         <v>905</v>
       </c>
-      <c r="B342" s="32" t="s">
+      <c r="C342" s="55" t="s">
         <v>906</v>
-      </c>
-      <c r="C342" s="55" t="s">
-        <v>907</v>
       </c>
       <c r="D342" s="32"/>
       <c r="E342" s="36" t="s">
@@ -11483,10 +11483,10 @@
     </row>
     <row r="343" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A343" s="32" t="s">
+        <v>907</v>
+      </c>
+      <c r="B343" s="32" t="s">
         <v>908</v>
-      </c>
-      <c r="B343" s="32" t="s">
-        <v>909</v>
       </c>
       <c r="C343" s="32"/>
       <c r="D343" s="32"/>
@@ -11502,10 +11502,10 @@
     </row>
     <row r="344" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A344" s="32" t="s">
+        <v>909</v>
+      </c>
+      <c r="B344" s="32" t="s">
         <v>910</v>
-      </c>
-      <c r="B344" s="32" t="s">
-        <v>911</v>
       </c>
       <c r="C344" s="32"/>
       <c r="D344" s="32"/>
@@ -11521,10 +11521,10 @@
     </row>
     <row r="345" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A345" s="32" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B345" s="32" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C345" s="32"/>
       <c r="D345" s="32"/>
@@ -11540,10 +11540,10 @@
     </row>
     <row r="346" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A346" s="64" t="s">
+        <v>912</v>
+      </c>
+      <c r="B346" s="64" t="s">
         <v>913</v>
-      </c>
-      <c r="B346" s="64" t="s">
-        <v>914</v>
       </c>
       <c r="C346" s="32"/>
       <c r="D346" s="32"/>
@@ -11559,10 +11559,10 @@
     </row>
     <row r="347" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A347" s="32" t="s">
+        <v>914</v>
+      </c>
+      <c r="B347" s="32" t="s">
         <v>915</v>
-      </c>
-      <c r="B347" s="32" t="s">
-        <v>916</v>
       </c>
       <c r="C347" s="32"/>
       <c r="D347" s="32"/>
@@ -11578,10 +11578,10 @@
     </row>
     <row r="348" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A348" s="32" t="s">
+        <v>916</v>
+      </c>
+      <c r="B348" s="32" t="s">
         <v>917</v>
-      </c>
-      <c r="B348" s="32" t="s">
-        <v>918</v>
       </c>
       <c r="C348" s="32"/>
       <c r="D348" s="32"/>
@@ -11597,10 +11597,10 @@
     </row>
     <row r="349" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A349" s="32" t="s">
+        <v>918</v>
+      </c>
+      <c r="B349" s="32" t="s">
         <v>919</v>
-      </c>
-      <c r="B349" s="32" t="s">
-        <v>920</v>
       </c>
       <c r="C349" s="32"/>
       <c r="D349" s="32"/>
@@ -11616,7 +11616,7 @@
     </row>
     <row r="350" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A350" s="32" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B350" s="32" t="s">
         <v>476</v>
@@ -11627,7 +11627,7 @@
         <v>18</v>
       </c>
       <c r="F350" s="8" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="G350" s="2"/>
       <c r="H350" s="2"/>
@@ -11635,10 +11635,10 @@
     </row>
     <row r="351" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A351" s="32" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B351" s="32" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C351" s="32"/>
       <c r="D351" s="32"/>
@@ -11657,7 +11657,7 @@
         <v>311</v>
       </c>
       <c r="B352" s="32" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C352" s="32"/>
       <c r="D352" s="32"/>
@@ -11673,7 +11673,7 @@
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A353" s="32" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B353" s="32" t="s">
         <v>552</v>
@@ -11692,10 +11692,10 @@
     </row>
     <row r="354" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A354" s="32" t="s">
+        <v>924</v>
+      </c>
+      <c r="B354" s="32" t="s">
         <v>925</v>
-      </c>
-      <c r="B354" s="32" t="s">
-        <v>926</v>
       </c>
       <c r="C354" s="32"/>
       <c r="D354" s="32"/>
@@ -11711,13 +11711,13 @@
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A355" s="32" t="s">
+        <v>926</v>
+      </c>
+      <c r="B355" s="32" t="s">
         <v>927</v>
       </c>
-      <c r="B355" s="32" t="s">
+      <c r="C355" s="55" t="s">
         <v>928</v>
-      </c>
-      <c r="C355" s="55" t="s">
-        <v>929</v>
       </c>
       <c r="D355" s="32">
         <v>6306968371</v>
@@ -11734,13 +11734,13 @@
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A356" s="32" t="s">
+        <v>929</v>
+      </c>
+      <c r="B356" s="32" t="s">
         <v>930</v>
       </c>
-      <c r="B356" s="32" t="s">
+      <c r="C356" s="55" t="s">
         <v>931</v>
-      </c>
-      <c r="C356" s="55" t="s">
-        <v>932</v>
       </c>
       <c r="D356" s="32">
         <v>9015908973</v>
@@ -11760,10 +11760,10 @@
         <v>238</v>
       </c>
       <c r="B357" s="32" t="s">
+        <v>932</v>
+      </c>
+      <c r="C357" s="55" t="s">
         <v>933</v>
-      </c>
-      <c r="C357" s="55" t="s">
-        <v>934</v>
       </c>
       <c r="D357" s="32">
         <v>3177039916</v>
@@ -11783,10 +11783,10 @@
         <v>273</v>
       </c>
       <c r="B358" s="32" t="s">
+        <v>934</v>
+      </c>
+      <c r="C358" s="55" t="s">
         <v>935</v>
-      </c>
-      <c r="C358" s="55" t="s">
-        <v>936</v>
       </c>
       <c r="D358" s="32">
         <v>8132299950</v>
@@ -11803,13 +11803,13 @@
     </row>
     <row r="359" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A359" s="32" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B359" s="32" t="s">
+        <v>936</v>
+      </c>
+      <c r="C359" s="55" t="s">
         <v>937</v>
-      </c>
-      <c r="C359" s="55" t="s">
-        <v>938</v>
       </c>
       <c r="D359" s="32"/>
       <c r="E359" s="8" t="s">
@@ -11824,13 +11824,13 @@
     </row>
     <row r="360" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A360" s="32" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B360" s="32" t="s">
         <v>399</v>
       </c>
       <c r="C360" s="55" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D360" s="32"/>
       <c r="E360" s="7" t="s">
@@ -11845,13 +11845,13 @@
     </row>
     <row r="361" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A361" s="32" t="s">
+        <v>940</v>
+      </c>
+      <c r="B361" s="32" t="s">
         <v>941</v>
       </c>
-      <c r="B361" s="32" t="s">
+      <c r="C361" s="55" t="s">
         <v>942</v>
-      </c>
-      <c r="C361" s="55" t="s">
-        <v>943</v>
       </c>
       <c r="D361" s="32">
         <v>8175042238</v>
@@ -11868,13 +11868,13 @@
     </row>
     <row r="362" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A362" s="32" t="s">
+        <v>943</v>
+      </c>
+      <c r="B362" s="32" t="s">
         <v>944</v>
       </c>
-      <c r="B362" s="32" t="s">
+      <c r="C362" s="55" t="s">
         <v>945</v>
-      </c>
-      <c r="C362" s="55" t="s">
-        <v>946</v>
       </c>
       <c r="D362" s="32">
         <v>8144230976</v>
@@ -11891,13 +11891,13 @@
     </row>
     <row r="363" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A363" s="32" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B363" s="32" t="s">
         <v>62</v>
       </c>
       <c r="C363" s="65" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D363" s="32"/>
       <c r="E363" s="7" t="s">
@@ -11912,13 +11912,13 @@
     </row>
     <row r="364" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A364" s="32" t="s">
+        <v>948</v>
+      </c>
+      <c r="B364" s="32" t="s">
         <v>949</v>
       </c>
-      <c r="B364" s="32" t="s">
+      <c r="C364" s="55" t="s">
         <v>950</v>
-      </c>
-      <c r="C364" s="55" t="s">
-        <v>951</v>
       </c>
       <c r="D364" s="32">
         <v>4254696275</v>
@@ -11938,10 +11938,10 @@
         <v>300</v>
       </c>
       <c r="B365" s="32" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C365" s="65" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="D365" s="32"/>
       <c r="E365" s="8" t="s">
@@ -11956,7 +11956,7 @@
     </row>
     <row r="366" spans="1:9" x14ac:dyDescent="0.75">
       <c r="A366" s="32" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B366" s="32" t="s">
         <v>661</v>
@@ -12101,6 +12101,7 @@
     <hyperlink ref="C363" r:id="rId110" xr:uid="{DE452F2F-221B-4BB0-A62D-39CA43701943}"/>
     <hyperlink ref="C364" r:id="rId111" xr:uid="{5E40AC15-C5F9-4A4F-8554-1ABA96BF95F0}"/>
     <hyperlink ref="C365" r:id="rId112" xr:uid="{D777BC4B-472E-4762-80CE-EA80476B691D}"/>
+    <hyperlink ref="C251" r:id="rId113" xr:uid="{03EA820A-6D1F-4E98-AD6D-9B101337E1C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>